<commit_message>
Add Modules Define on Sheet 2
</commit_message>
<xml_diff>
--- a/docs/User Requirements.xlsx
+++ b/docs/User Requirements.xlsx
@@ -9,11 +9,16 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7335"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7335" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$2:$I$32</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$B$2:$B$44</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -24,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="96">
   <si>
     <t>User</t>
   </si>
@@ -47,9 +52,6 @@
     <t>High</t>
   </si>
   <si>
-    <t>Admin</t>
-  </si>
-  <si>
     <t>ROLE_ADMIN</t>
   </si>
   <si>
@@ -65,12 +67,6 @@
     <t>Dapat menambah, mengubah, menghapus dan melihat seluruh mata kuliah</t>
   </si>
   <si>
-    <t>Mahasiswa</t>
-  </si>
-  <si>
-    <t>Dosen</t>
-  </si>
-  <si>
     <t>Account</t>
   </si>
   <si>
@@ -89,9 +85,6 @@
     <t>ROLE_TU</t>
   </si>
   <si>
-    <t>Tata Usaha</t>
-  </si>
-  <si>
     <t>Dapat menambah, mengubah, menghapus dan melihat semua akun untuk mahasiswa</t>
   </si>
   <si>
@@ -137,18 +130,6 @@
     <t>Untuk hak akses admin, dapat mengakses seluruh modul. Pembuatan username secara default mengambil data dari identity_number setiap akun yang dibuat. Untuk fungsi delete bukan menghapus data pada tabel tetapi hanya mengubah status is_deleted menjadi false.</t>
   </si>
   <si>
-    <t>Laboran</t>
-  </si>
-  <si>
-    <t>ROLE_LABORAN</t>
-  </si>
-  <si>
-    <t>Dapat memverifikasi atau aktivasi mahasiswa yang mendaftar praktikum sesuai slot nya</t>
-  </si>
-  <si>
-    <t>Dapat menambah, mengubah, menghapus dan melihat jadwal atau slot praktikum</t>
-  </si>
-  <si>
     <t>Dapat melihat data mahasiswa yang mengambil praktikum berdasarkan mata kuliah yang diampu</t>
   </si>
   <si>
@@ -173,18 +154,6 @@
     <t>Dapat melihat nilai mata kuliah yang diambil</t>
   </si>
   <si>
-    <t>Dapat melihat praktikum yang di tawarkan pada semester yang berjalan</t>
-  </si>
-  <si>
-    <t>Dapat mengambil slot praktikum yang di tawarkan pada semester yang berjalan sesuai mata kuliah yang diambil</t>
-  </si>
-  <si>
-    <t>Dapat melihat nilai praktikum yang diambil</t>
-  </si>
-  <si>
-    <t>System</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
@@ -194,27 +163,15 @@
     <t>Dapat memiliki fitur pencarian pada daftar (mahasiswa, dosen, laboran, mata kuliah, praktikum, jadwal kuliah) sesuai role masing-masing akun</t>
   </si>
   <si>
-    <t>Untuk fungsi delete bukan menghapus data pada tabel tetapi hanya mengubah status is_deleted menjadi false.</t>
-  </si>
-  <si>
     <t>Nilai menggunakan angka</t>
   </si>
   <si>
-    <t>Dapat melihat mata kuliah yang memiliki praktikum</t>
-  </si>
-  <si>
-    <t>Proses aktivasi hanya mengubah status is_active menjadi True atau 1</t>
-  </si>
-  <si>
     <t>Dapat memilih beberapa mata kuliah dalam sekali pengambilan mata kuliah (menggunakan array)</t>
   </si>
   <si>
     <t>Nilai yang ditampilkan adalah hasil konversi dari angka menjadi huruf</t>
   </si>
   <si>
-    <t>Dapat memilih beberapa praktikum dalam sekali pengambilan slot (menggunakan array)</t>
-  </si>
-  <si>
     <t>Disajikan dalam bentuk tabel untuk penyajian data (menggunakan datatables.js dan customisasi key pencarian di javascript)</t>
   </si>
   <si>
@@ -236,9 +193,6 @@
     <t>Random string dan angka</t>
   </si>
   <si>
-    <t>All Module</t>
-  </si>
-  <si>
     <t>Database Name</t>
   </si>
   <si>
@@ -252,6 +206,117 @@
   </si>
   <si>
     <t>Password</t>
+  </si>
+  <si>
+    <t>Search</t>
+  </si>
+  <si>
+    <t>Auth Required</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Feature</t>
+  </si>
+  <si>
+    <t>Add User</t>
+  </si>
+  <si>
+    <t>Edit User</t>
+  </si>
+  <si>
+    <t>Delete User</t>
+  </si>
+  <si>
+    <t>Update Password</t>
+  </si>
+  <si>
+    <t>Edit Program Study</t>
+  </si>
+  <si>
+    <t>Add Program Study</t>
+  </si>
+  <si>
+    <t>Edit Course</t>
+  </si>
+  <si>
+    <t>Dependent</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Update</t>
+  </si>
+  <si>
+    <t>Take Class</t>
+  </si>
+  <si>
+    <t>Make Class</t>
+  </si>
+  <si>
+    <t>Scheduler</t>
+  </si>
+  <si>
+    <t>Edit Schedule</t>
+  </si>
+  <si>
+    <t>Disable Account</t>
+  </si>
+  <si>
+    <t>Disable Program Study</t>
+  </si>
+  <si>
+    <t>Disable Schedule</t>
+  </si>
+  <si>
+    <t>Absent</t>
+  </si>
+  <si>
+    <t>Make Absent</t>
+  </si>
+  <si>
+    <t>Read Absent</t>
+  </si>
+  <si>
+    <t>Add Score</t>
+  </si>
+  <si>
+    <t>Disable Course</t>
+  </si>
+  <si>
+    <t>Class, Department</t>
+  </si>
+  <si>
+    <t>Courses, Class</t>
+  </si>
+  <si>
+    <t>Class, Department, Account</t>
+  </si>
+  <si>
+    <t>Courses Class</t>
+  </si>
+  <si>
+    <t>Scheduler, Class, Courses</t>
+  </si>
+  <si>
+    <t>Read Scheduler</t>
+  </si>
+  <si>
+    <t>Make Scheduler</t>
+  </si>
+  <si>
+    <t>Read Course</t>
+  </si>
+  <si>
+    <t>Make Course</t>
   </si>
 </sst>
 </file>
@@ -289,7 +354,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -347,23 +412,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -378,14 +432,32 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -401,12 +473,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -689,16 +755,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:L38"/>
+  <dimension ref="B2:L32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30:XFD32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.140625" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" customWidth="1"/>
     <col min="3" max="3" width="21.140625" customWidth="1"/>
     <col min="4" max="4" width="71.85546875" style="1" customWidth="1"/>
     <col min="5" max="5" width="34" style="1" customWidth="1"/>
@@ -709,39 +775,39 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B2" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="10" t="s">
+      <c r="B2" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="K2" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="L2" s="14" t="s">
-        <v>72</v>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="K2" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="2:12" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
       <c r="G3" s="2" t="s">
         <v>4</v>
       </c>
@@ -751,649 +817,1193 @@
       <c r="I3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="K3" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="L3" s="14" t="s">
-        <v>74</v>
+      <c r="K3" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="2:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>8</v>
-      </c>
       <c r="D4" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>36</v>
+        <v>18</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>32</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
       <c r="I4" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="L4" s="8"/>
+    </row>
+    <row r="5" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="B5" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="K4" s="14" t="s">
-        <v>75</v>
-      </c>
-      <c r="L4" s="15"/>
-    </row>
-    <row r="5" spans="2:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" s="9"/>
+      <c r="E5" s="15"/>
       <c r="F5" s="4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
       <c r="I5" s="5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="2:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
+      <c r="B6" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>7</v>
+      </c>
       <c r="D6" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6" s="9"/>
+        <v>20</v>
+      </c>
+      <c r="E6" s="15"/>
       <c r="F6" s="4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
       <c r="I6" s="5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="2:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
+      <c r="B7" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>7</v>
+      </c>
       <c r="D7" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E7" s="9"/>
+        <v>21</v>
+      </c>
+      <c r="E7" s="15"/>
       <c r="F7" s="4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
       <c r="I7" s="5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="2:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
+      <c r="B8" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>7</v>
+      </c>
       <c r="D8" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E8" s="9"/>
+        <v>22</v>
+      </c>
+      <c r="E8" s="15"/>
       <c r="F8" s="4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
       <c r="I8" s="5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="2:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
+      <c r="B9" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>7</v>
+      </c>
       <c r="D9" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" s="9"/>
+        <v>10</v>
+      </c>
+      <c r="E9" s="15"/>
       <c r="F9" s="4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
       <c r="I9" s="5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="2:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
+      <c r="B10" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>7</v>
+      </c>
       <c r="D10" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10" s="9"/>
+        <v>11</v>
+      </c>
+      <c r="E10" s="15"/>
       <c r="F10" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
       <c r="I10" s="5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="2:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
+      <c r="B11" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>7</v>
+      </c>
       <c r="D11" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E11" s="9"/>
+        <v>25</v>
+      </c>
+      <c r="E11" s="15"/>
       <c r="F11" s="4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
       <c r="I11" s="5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="2:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="B12" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>20</v>
+      <c r="B12" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>17</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E12" s="9" t="s">
-        <v>64</v>
+        <v>18</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>48</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
       <c r="I12" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="B13" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="13" spans="2:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E13" s="9"/>
+      <c r="E13" s="15"/>
       <c r="F13" s="4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
       <c r="I13" s="5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="2:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
+      <c r="B14" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>17</v>
+      </c>
       <c r="D14" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E14" s="9"/>
+        <v>23</v>
+      </c>
+      <c r="E14" s="15"/>
       <c r="F14" s="4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
       <c r="I14" s="5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="2:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
+      <c r="B15" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>17</v>
+      </c>
       <c r="D15" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E15" s="9"/>
+        <v>22</v>
+      </c>
+      <c r="E15" s="15"/>
       <c r="F15" s="4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
       <c r="I15" s="5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="2:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
+      <c r="B16" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>17</v>
+      </c>
       <c r="D16" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E16" s="9"/>
+        <v>30</v>
+      </c>
+      <c r="E16" s="15"/>
       <c r="F16" s="4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
       <c r="I16" s="5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="2:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
+      <c r="B17" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>17</v>
+      </c>
       <c r="D17" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E17" s="9"/>
+        <v>11</v>
+      </c>
+      <c r="E17" s="15"/>
       <c r="F17" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
       <c r="I17" s="5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="2:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
+      <c r="B18" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>17</v>
+      </c>
       <c r="D18" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E18" s="9"/>
+        <v>24</v>
+      </c>
+      <c r="E18" s="15"/>
       <c r="F18" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
       <c r="I18" s="5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="2:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
+      <c r="B19" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>17</v>
+      </c>
       <c r="D19" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E19" s="9"/>
+        <v>26</v>
+      </c>
+      <c r="E19" s="15"/>
       <c r="F19" s="4" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
       <c r="I19" s="5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="2:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
+      <c r="B20" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>17</v>
+      </c>
       <c r="D20" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="E20" s="9"/>
+        <v>37</v>
+      </c>
+      <c r="E20" s="15"/>
       <c r="F20" s="4" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
       <c r="I20" s="5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="21" spans="2:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B21" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>31</v>
+      <c r="B21" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>27</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E21" s="4"/>
       <c r="F21" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
     </row>
     <row r="22" spans="2:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
+      <c r="B22" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>27</v>
+      </c>
       <c r="D22" s="4" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
       <c r="G22" s="3"/>
       <c r="H22" s="5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="I22" s="3"/>
     </row>
     <row r="23" spans="2:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
+      <c r="B23" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>27</v>
+      </c>
       <c r="D23" s="4" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E23" s="4"/>
       <c r="F23" s="4" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
     </row>
     <row r="24" spans="2:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
+      <c r="B24" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>27</v>
+      </c>
       <c r="D24" s="4" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="E24" s="4"/>
       <c r="F24" s="4" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="H24" s="3"/>
       <c r="I24" s="3"/>
     </row>
     <row r="25" spans="2:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="B25" s="8"/>
-      <c r="C25" s="8"/>
+      <c r="B25" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>27</v>
+      </c>
       <c r="D25" s="4" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="G25" s="3"/>
       <c r="H25" s="5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="I25" s="3"/>
     </row>
     <row r="26" spans="2:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B26" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>38</v>
+      <c r="B26" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>35</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>58</v>
+        <v>36</v>
       </c>
       <c r="E26" s="4"/>
       <c r="F26" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="H26" s="3"/>
       <c r="I26" s="3"/>
     </row>
-    <row r="27" spans="2:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="B27" s="7"/>
-      <c r="C27" s="7"/>
+    <row r="27" spans="2:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="B27" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>35</v>
+      </c>
       <c r="D27" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>18</v>
+        <v>49</v>
       </c>
       <c r="G27" s="3"/>
-      <c r="H27" s="3"/>
-      <c r="I27" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="28" spans="2:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="B28" s="8"/>
-      <c r="C28" s="8"/>
+      <c r="H27" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I27" s="3"/>
+    </row>
+    <row r="28" spans="2:9" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B28" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>35</v>
+      </c>
       <c r="D28" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="E28" s="4" t="s">
-        <v>59</v>
-      </c>
+      <c r="E28" s="4"/>
       <c r="F28" s="4" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="H28" s="3"/>
       <c r="I28" s="3"/>
     </row>
-    <row r="29" spans="2:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B29" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C29" s="6" t="s">
-        <v>43</v>
+    <row r="29" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="B29" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>35</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="E29" s="4"/>
+        <v>40</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>46</v>
+      </c>
       <c r="F29" s="4" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="H29" s="3"/>
       <c r="I29" s="3"/>
     </row>
-    <row r="30" spans="2:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="B30" s="7"/>
-      <c r="C30" s="7"/>
+    <row r="30" spans="2:9" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B30" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>41</v>
+      </c>
       <c r="D30" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>60</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="E30" s="4"/>
       <c r="F30" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="G30" s="3"/>
-      <c r="H30" s="5" t="s">
-        <v>19</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="G30" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H30" s="3"/>
       <c r="I30" s="3"/>
     </row>
-    <row r="31" spans="2:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B31" s="7"/>
-      <c r="C31" s="7"/>
+    <row r="31" spans="2:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="B31" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>41</v>
+      </c>
       <c r="D31" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E31" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="E31" s="4"/>
       <c r="F31" s="4" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="H31" s="3"/>
       <c r="I31" s="3"/>
     </row>
     <row r="32" spans="2:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="B32" s="7"/>
-      <c r="C32" s="7"/>
+      <c r="B32" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>41</v>
+      </c>
       <c r="D32" s="4" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="G32" s="5" t="s">
-        <v>19</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="G32" s="3"/>
       <c r="H32" s="3"/>
-      <c r="I32" s="3"/>
-    </row>
-    <row r="33" spans="2:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B33" s="7"/>
-      <c r="C33" s="7"/>
-      <c r="D33" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="E33" s="4"/>
-      <c r="F33" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="G33" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H33" s="3"/>
-      <c r="I33" s="3"/>
-    </row>
-    <row r="34" spans="2:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="B34" s="7"/>
-      <c r="C34" s="7"/>
-      <c r="D34" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="E34" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="F34" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="G34" s="3"/>
-      <c r="H34" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="I34" s="3"/>
-    </row>
-    <row r="35" spans="2:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="B35" s="8"/>
-      <c r="C35" s="8"/>
-      <c r="D35" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="E35" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="F35" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="G35" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H35" s="3"/>
-      <c r="I35" s="3"/>
-    </row>
-    <row r="36" spans="2:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B36" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="C36" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D36" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="E36" s="4"/>
-      <c r="F36" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G36" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H36" s="3"/>
-      <c r="I36" s="3"/>
-    </row>
-    <row r="37" spans="2:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="B37" s="7"/>
-      <c r="C37" s="7"/>
-      <c r="D37" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="E37" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="F37" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="G37" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H37" s="3"/>
-      <c r="I37" s="3"/>
-    </row>
-    <row r="38" spans="2:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="B38" s="8"/>
-      <c r="C38" s="8"/>
-      <c r="D38" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="E38" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="F38" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="G38" s="3"/>
-      <c r="H38" s="3"/>
-      <c r="I38" s="5" t="s">
-        <v>19</v>
+      <c r="I32" s="5" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="20">
+  <mergeCells count="8">
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="E4:E11"/>
+    <mergeCell ref="E12:E20"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="D2:D3"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="C36:C38"/>
-    <mergeCell ref="B36:B38"/>
-    <mergeCell ref="C29:C35"/>
-    <mergeCell ref="B29:B35"/>
-    <mergeCell ref="C26:C28"/>
-    <mergeCell ref="B26:B28"/>
-    <mergeCell ref="C21:C25"/>
-    <mergeCell ref="B21:B25"/>
-    <mergeCell ref="C12:C20"/>
-    <mergeCell ref="B12:B20"/>
-    <mergeCell ref="E4:E11"/>
-    <mergeCell ref="E12:E20"/>
-    <mergeCell ref="C4:C11"/>
-    <mergeCell ref="B4:B11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:H25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.140625" customWidth="1"/>
+    <col min="2" max="2" width="23.140625" customWidth="1"/>
+    <col min="3" max="3" width="28" customWidth="1"/>
+    <col min="4" max="4" width="23.140625" customWidth="1"/>
+    <col min="5" max="5" width="22.5703125" style="12" customWidth="1"/>
+    <col min="6" max="7" width="18.42578125" style="12" customWidth="1"/>
+    <col min="8" max="8" width="21.42578125" style="12" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" s="17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="H4" s="13" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="H5" s="13" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="G6" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="H6" s="13" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B7" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="G7" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="H7" s="13" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B8" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="G8" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="H8" s="13" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="G9" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="H9" s="13" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="F10" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="G10" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="H10" s="13" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B11" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="G11" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="H11" s="13" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B12" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="F12" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="G12" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="H12" s="13" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B13" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="H13" s="13" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B14" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="F14" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="G14" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="H14" s="13" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B15" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="F15" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="G15" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="H15" s="13" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B16" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="F16" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="G16" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="H16" s="13" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B17" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="E17" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="F17" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="G17" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="H17" s="13" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B18" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="E18" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="F18" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="G18" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="H18" s="13" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B19" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="E19" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="F19" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="G19" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="H19" s="13" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B20" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="E20" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="F20" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="G20" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="H20" s="13" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B21" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="E21" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="F21" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="G21" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="H21" s="13" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B22" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="E22" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="F22" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="G22" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="H22" s="13" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B23" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="E23" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="F23" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="G23" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="H23" s="13" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B24" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="E24" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="F24" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="G24" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="H24" s="13" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B25" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="E25" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="F25" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="G25" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="H25" s="13" t="s">
+        <v>73</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="B2:B44"/>
+  <mergeCells count="7">
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>